<commit_message>
enhace script for importing major
</commit_message>
<xml_diff>
--- a/db/csv/personality_category.xlsx
+++ b/db/csv/personality_category.xlsx
@@ -3,15 +3,31 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Personality" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="D1">
+      <text>
+        <t xml:space="preserve">ចំពោះ description សូមដាក់ (;) ដើម្បីផ្តាច់ list item ពីគ្នា
+	-Sokly Heng</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>code</t>
   </si>
@@ -22,15 +38,12 @@
     <t>name_km</t>
   </si>
   <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>category</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>real001</t>
   </si>
   <si>
@@ -40,13 +53,14 @@
     <t>ប្រាកដនិយម</t>
   </si>
   <si>
+    <t>ធ្វើការដោយការអនុវត្តជាក់ស្តែង;
+ធ្វើការដោយប្រើម៉ាស៊ីន ឬសម្ភារៈឧបទ្ទេស;
+ធ្វើការដោយប្រើសត្វជាកម្លាំងជំនួយ;
+ធ្វើការដោយប្រើកម្លាំងជាមធ្យោបាយ;
+ធ្វើការជាអ្នកបើកបរ</t>
+  </si>
+  <si>
     <t>science</t>
-  </si>
-  <si>
-    <t>ធ្វើការដោយការអនុវត្តជាក់ស្តែង;ធ្វើការដោយប្រើម៉ាស៊ីន ឬសម្ភារៈឧបទ្ទេស;ធ្វើការដោយប្រើសត្វជាកម្លាំងជំនួយ;ធ្វើការដោយប្រើកម្លាំងជាមធ្យោបាយ;ធ្វើការជាអ្នកបើកបរ</t>
-  </si>
-  <si>
-    <t>ចំពោះ description សូមដាក់ (;) ដើម្បីផ្តាច់ list item ពីគ្នា</t>
   </si>
   <si>
     <t>inv001</t>
@@ -109,18 +123,12 @@
     </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,14 +137,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -147,9 +155,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -173,7 +178,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="41.29"/>
+    <col customWidth="1" min="4" max="4" width="41.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -192,30 +197,26 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -235,23 +236,22 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
       <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -274,22 +274,21 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -311,22 +310,21 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
       <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -348,22 +346,21 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
       <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -385,23 +382,22 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
       <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -424,9 +420,9 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
       <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>